<commit_message>
Unlock cells in SBH-FORM-2 for the end user to fill in
</commit_message>
<xml_diff>
--- a/creator/forms_xlsx/SBH-FORM.xlsx
+++ b/creator/forms_xlsx/SBH-FORM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bprc_project\VM\tbpc_dev\tbpc\resource_mgt\forms_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo_dev\extra_addons\budget_outsource\creator\forms_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SBH-FORM 1" sheetId="1" r:id="rId1"/>
@@ -217,9 +217,6 @@
     <t>Period of Delay by (weeks)</t>
   </si>
   <si>
-    <t>Delay Penalty (2% max)</t>
-  </si>
-  <si>
     <t>Apply Penalty</t>
   </si>
   <si>
@@ -267,6 +264,10 @@
   </si>
   <si>
     <t>Head Of Division (VP/SVP)</t>
+  </si>
+  <si>
+    <t>Delay Penalty 
+(2% max)</t>
   </si>
 </sst>
 </file>
@@ -904,7 +905,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -924,9 +925,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -945,17 +943,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1027,9 +1019,6 @@
     <xf numFmtId="43" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1213,6 +1202,25 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1277,11 +1285,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1331,8 +1341,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1355,26 +1374,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1401,9 +1426,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1693,656 +1715,656 @@
   </sheetPr>
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2" style="81" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="81" customWidth="1"/>
-    <col min="3" max="4" width="10.7109375" style="81" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="81" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="81" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="81" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="81" customWidth="1"/>
-    <col min="9" max="9" width="10" style="81" customWidth="1"/>
-    <col min="10" max="11" width="12.7109375" style="81" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="81" customWidth="1"/>
-    <col min="13" max="14" width="26.42578125" style="81" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" style="81" customWidth="1"/>
-    <col min="16" max="16" width="2" style="81" customWidth="1"/>
-    <col min="17" max="17" width="32" style="81" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="9.140625" style="81" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="77" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="77" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" style="77" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="77" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="77" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="77" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="77" customWidth="1"/>
+    <col min="9" max="9" width="10" style="77" customWidth="1"/>
+    <col min="10" max="11" width="12.7109375" style="77" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="77" customWidth="1"/>
+    <col min="13" max="14" width="26.42578125" style="77" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" style="77" customWidth="1"/>
+    <col min="16" max="16" width="2" style="77" customWidth="1"/>
+    <col min="17" max="17" width="32" style="77" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="77" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="81" hidden="1" customWidth="1"/>
-    <col min="22" max="25" width="0" style="81" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="81" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="81"/>
+    <col min="21" max="21" width="9.140625" style="77" hidden="1" customWidth="1"/>
+    <col min="22" max="25" width="0" style="77" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="77" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="36"/>
+      <c r="B1" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="33"/>
     </row>
     <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
-      <c r="P2" s="36"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="33"/>
     </row>
     <row r="3" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P3" s="36"/>
-      <c r="Y3" s="66"/>
+      <c r="P3" s="33"/>
+      <c r="Y3" s="62"/>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="98"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="36"/>
-      <c r="T4" s="81"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="33"/>
+      <c r="T4" s="77"/>
       <c r="V4"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85" t="s">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="83">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="T5" s="77"/>
+      <c r="V5"/>
+    </row>
+    <row r="6" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="27"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="33"/>
+      <c r="T6" s="77"/>
+      <c r="V6"/>
+    </row>
+    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="97" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="83">
+        <v>0</v>
+      </c>
+      <c r="K7" s="46"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="33"/>
+      <c r="T7" s="77"/>
+      <c r="V7"/>
+    </row>
+    <row r="8" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="33"/>
+      <c r="T8" s="77"/>
+      <c r="V8"/>
+    </row>
+    <row r="9" spans="1:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Y9" s="62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="127" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="121"/>
+      <c r="L10" s="121"/>
+      <c r="M10" s="121"/>
+      <c r="N10" s="121"/>
+      <c r="O10" s="121"/>
+      <c r="P10" s="33"/>
+      <c r="Y10" s="62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="130"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="131"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="132"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="122"/>
+      <c r="M11" s="122"/>
+      <c r="N11" s="122"/>
+      <c r="O11" s="122"/>
+      <c r="P11" s="33"/>
+      <c r="Y11" s="62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="133" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="134"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="134"/>
+      <c r="H12" s="134"/>
+      <c r="I12" s="134"/>
+      <c r="J12" s="134"/>
+      <c r="K12" s="134"/>
+      <c r="L12" s="134"/>
+      <c r="M12" s="134"/>
+      <c r="N12" s="135"/>
+      <c r="O12" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="33"/>
+      <c r="Y12" s="62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="92" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="92" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="101" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="87">
-        <v>0</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="T5" s="81"/>
-      <c r="V5"/>
-    </row>
-    <row r="6" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="30"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="36"/>
-      <c r="T6" s="81"/>
-      <c r="V6"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="101" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="87">
-        <v>0</v>
-      </c>
-      <c r="K7" s="50"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="36"/>
-      <c r="T7" s="81"/>
-      <c r="V7"/>
-    </row>
-    <row r="8" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="36"/>
-      <c r="T8" s="81"/>
-      <c r="V8"/>
-    </row>
-    <row r="9" spans="1:25" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Y9" s="66" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="126" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="127"/>
-      <c r="D10" s="127"/>
-      <c r="E10" s="127"/>
-      <c r="F10" s="127"/>
-      <c r="G10" s="127"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="120" t="s">
-        <v>76</v>
-      </c>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="120"/>
-      <c r="O10" s="120"/>
-      <c r="P10" s="36"/>
-      <c r="Y10" s="66" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="129"/>
-      <c r="C11" s="130"/>
-      <c r="D11" s="130"/>
-      <c r="E11" s="130"/>
-      <c r="F11" s="130"/>
-      <c r="G11" s="130"/>
-      <c r="H11" s="130"/>
-      <c r="I11" s="131"/>
-      <c r="J11" s="121"/>
-      <c r="K11" s="121"/>
-      <c r="L11" s="121"/>
-      <c r="M11" s="121"/>
-      <c r="N11" s="121"/>
-      <c r="O11" s="121"/>
-      <c r="P11" s="36"/>
-      <c r="Y11" s="66" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="132" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
-      <c r="L12" s="133"/>
-      <c r="M12" s="133"/>
-      <c r="N12" s="134"/>
-      <c r="O12" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="P12" s="36"/>
-      <c r="Y12" s="66" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="96" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="96" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="96" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="96" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="96" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="96" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="96" t="s">
+      <c r="J13" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="96" t="s">
+      <c r="K13" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="96" t="s">
+      <c r="L13" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="96" t="s">
+      <c r="M13" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="N13" s="96" t="s">
+      <c r="N13" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="O13" s="96" t="s">
+      <c r="O13" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="83" t="str">
+      <c r="P13" s="33"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="79" t="str">
         <f t="shared" ref="R13:R15" si="0">G13</f>
         <v>Level</v>
       </c>
-      <c r="S13" s="83" t="str">
+      <c r="S13" s="79" t="str">
         <f t="shared" ref="S13:S15" si="1">K13</f>
         <v xml:space="preserve">Total Delivered No. of Hours in a Month </v>
       </c>
-      <c r="T13" s="83" t="str">
+      <c r="T13" s="79" t="str">
         <f t="shared" ref="T13:T15" si="2">L13</f>
         <v>Tools &amp; Uniform Deduction
 Yes / Blank</v>
       </c>
-      <c r="Y13" s="66" t="s">
+      <c r="Y13" s="62" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="66" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="70"/>
-      <c r="N14" s="70"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="66" t="str">
+    <row r="14" spans="1:25" s="62" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="64"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="62" t="str">
         <f>CONCATENATE(C14," ",F14)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="R14" s="66">
+      <c r="R14" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S14" s="66">
+      <c r="S14" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T14" s="66">
+      <c r="T14" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y14" s="66" t="s">
+      <c r="Y14" s="62" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" s="66" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="68">
-        <v>0</v>
-      </c>
-      <c r="C15" s="69">
+    <row r="15" spans="1:25" s="62" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="64">
+        <v>0</v>
+      </c>
+      <c r="C15" s="65">
         <v>1</v>
       </c>
-      <c r="D15" s="69">
+      <c r="D15" s="65">
         <v>2</v>
       </c>
-      <c r="E15" s="82">
+      <c r="E15" s="78">
         <v>3</v>
       </c>
-      <c r="F15" s="69">
+      <c r="F15" s="65">
         <v>4</v>
       </c>
-      <c r="G15" s="69">
+      <c r="G15" s="65">
         <v>5</v>
       </c>
-      <c r="H15" s="69">
+      <c r="H15" s="65">
         <v>6</v>
       </c>
-      <c r="I15" s="69">
+      <c r="I15" s="65">
         <v>7</v>
       </c>
-      <c r="J15" s="69">
+      <c r="J15" s="65">
         <v>8</v>
       </c>
-      <c r="K15" s="177">
+      <c r="K15" s="110">
         <v>9</v>
       </c>
-      <c r="L15" s="69">
+      <c r="L15" s="65">
         <v>10</v>
       </c>
-      <c r="M15" s="177">
+      <c r="M15" s="110">
         <v>11</v>
       </c>
-      <c r="N15" s="177">
+      <c r="N15" s="110">
         <v>12</v>
       </c>
-      <c r="O15" s="177">
+      <c r="O15" s="110">
         <v>13</v>
       </c>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="66" t="str">
+      <c r="P15" s="63"/>
+      <c r="Q15" s="62" t="str">
         <f t="shared" ref="Q15:Q20" si="3">CONCATENATE(C15," ",F15, " ",I15)</f>
         <v>1 4 7</v>
       </c>
-      <c r="R15" s="66">
+      <c r="R15" s="62">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="S15" s="66">
+      <c r="S15" s="62">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="T15" s="66">
+      <c r="T15" s="62">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="Y15" s="66" t="s">
+      <c r="Y15" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="27"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="66" t="str">
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="62" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="R16" s="66">
+      <c r="R16" s="62">
         <f t="shared" ref="R16:R20" si="4">G16</f>
         <v>0</v>
       </c>
-      <c r="S16" s="66">
+      <c r="S16" s="62">
         <f t="shared" ref="S16:S20" si="5">K16</f>
         <v>0</v>
       </c>
-      <c r="T16" s="66">
+      <c r="T16" s="62">
         <f t="shared" ref="T16:T20" si="6">L16</f>
         <v>0</v>
       </c>
-      <c r="Y16" s="66" t="s">
+      <c r="Y16" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="122" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="123"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="66" t="str">
+      <c r="F17" s="124"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="62" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="R17" s="66">
+      <c r="R17" s="62">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S17" s="66">
+      <c r="S17" s="62">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="T17" s="66">
+      <c r="T17" s="62">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y17" s="66" t="s">
+      <c r="Y17" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="33"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="66" t="str">
+      <c r="B18" s="30"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="62" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="R18" s="66">
+      <c r="R18" s="62">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S18" s="66">
+      <c r="S18" s="62">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="T18" s="66">
+      <c r="T18" s="62">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y18" s="66" t="s">
+      <c r="Y18" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="66" t="str">
+      <c r="B19" s="30"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="62" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="R19" s="66">
+      <c r="R19" s="62">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S19" s="66">
+      <c r="S19" s="62">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="T19" s="66">
+      <c r="T19" s="62">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y19" s="66" t="s">
+      <c r="Y19" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="25"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="93"/>
-      <c r="I20" s="93"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="93"/>
-      <c r="L20" s="93"/>
-      <c r="M20" s="93"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="93"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="66" t="str">
+      <c r="B20" s="22"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="89"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="62" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="R20" s="66">
+      <c r="R20" s="62">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S20" s="66">
+      <c r="S20" s="62">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="T20" s="66">
+      <c r="T20" s="62">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y20" s="66" t="s">
+      <c r="Y20" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="36"/>
-      <c r="Y21" s="66" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="33"/>
+      <c r="Y21" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="124"/>
-      <c r="B22" s="125"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="125"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
+      <c r="A22" s="125"/>
+      <c r="B22" s="126"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O22" s="3"/>
-      <c r="P22" s="36"/>
-      <c r="Y22" s="66" t="s">
+      <c r="P22" s="33"/>
+      <c r="Y22" s="62" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2351,88 +2373,88 @@
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="114" t="s">
+      <c r="B24" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="L24" s="105"/>
-      <c r="M24" s="102"/>
-      <c r="N24" s="102"/>
-      <c r="O24" s="102"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="115"/>
+      <c r="E24" s="115"/>
+      <c r="L24" s="101"/>
+      <c r="M24" s="98"/>
+      <c r="N24" s="98"/>
+      <c r="O24" s="98"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B25" s="115" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="115"/>
-      <c r="D25" s="115"/>
-      <c r="E25" s="115"/>
-      <c r="L25" s="105"/>
-      <c r="M25" s="104"/>
-      <c r="N25" s="104"/>
-      <c r="O25" s="104"/>
+      <c r="B25" s="116" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="L25" s="101"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="100"/>
       <c r="P25" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:25" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116"/>
-      <c r="L26" s="100"/>
-      <c r="M26" s="103"/>
-      <c r="N26" s="103"/>
-      <c r="O26" s="103"/>
-      <c r="T26" s="106"/>
+      <c r="B26" s="117" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="117"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="L26" s="96"/>
+      <c r="M26" s="99"/>
+      <c r="N26" s="99"/>
+      <c r="O26" s="99"/>
+      <c r="T26" s="102"/>
     </row>
     <row r="27" spans="1:25" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="116" t="s">
+      <c r="B27" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="116"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="L27" s="100"/>
-      <c r="M27" s="103"/>
-      <c r="N27" s="103"/>
-      <c r="O27" s="103"/>
-      <c r="T27" s="106"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="L27" s="96"/>
+      <c r="M27" s="99"/>
+      <c r="N27" s="99"/>
+      <c r="O27" s="99"/>
+      <c r="T27" s="102"/>
     </row>
     <row r="28" spans="1:25" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="116" t="s">
+      <c r="B28" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="116"/>
-      <c r="D28" s="116"/>
-      <c r="E28" s="116"/>
-      <c r="L28" s="100"/>
-      <c r="M28" s="103"/>
-      <c r="N28" s="103"/>
-      <c r="O28" s="103"/>
-      <c r="T28" s="106"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="99"/>
+      <c r="N28" s="99"/>
+      <c r="O28" s="99"/>
+      <c r="T28" s="102"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="89"/>
+      <c r="E29" s="85"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Q31" s="15"/>
+      <c r="Q31" s="13"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Q32" s="15"/>
+      <c r="Q32" s="13"/>
     </row>
     <row r="34" spans="6:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2465,892 +2487,892 @@
   </sheetPr>
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="81" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="81" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="81" customWidth="1"/>
-    <col min="4" max="6" width="5.7109375" style="81" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="81" customWidth="1"/>
-    <col min="8" max="9" width="5.7109375" style="81" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" style="81" customWidth="1"/>
-    <col min="13" max="15" width="16.5703125" style="45" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="81" customWidth="1"/>
-    <col min="17" max="17" width="1.5703125" style="81" customWidth="1"/>
-    <col min="18" max="20" width="7.140625" style="81" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="81" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" style="77" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="77" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="77" customWidth="1"/>
+    <col min="4" max="6" width="5.7109375" style="77" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="77" customWidth="1"/>
+    <col min="8" max="9" width="5.7109375" style="77" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="77" customWidth="1"/>
+    <col min="13" max="15" width="16.5703125" style="41" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" style="77" customWidth="1"/>
+    <col min="17" max="17" width="1.5703125" style="77" customWidth="1"/>
+    <col min="18" max="20" width="7.140625" style="77" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="77" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="23" max="26" width="9.140625" style="81" hidden="1" customWidth="1"/>
-    <col min="27" max="28" width="9.140625" style="81" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="81"/>
+    <col min="23" max="26" width="9.140625" style="77" hidden="1" customWidth="1"/>
+    <col min="27" max="28" width="9.140625" style="77" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="36"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="36"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="33"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="148" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="147"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="147"/>
-      <c r="K3" s="147"/>
-      <c r="L3" s="147"/>
-      <c r="M3" s="147"/>
-      <c r="N3" s="147"/>
-      <c r="O3" s="147"/>
-      <c r="P3" s="147"/>
-      <c r="Q3" s="36"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="148"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
+      <c r="K3" s="148"/>
+      <c r="L3" s="148"/>
+      <c r="M3" s="148"/>
+      <c r="N3" s="148"/>
+      <c r="O3" s="148"/>
+      <c r="P3" s="148"/>
+      <c r="Q3" s="33"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="85" t="str">
+      <c r="C4" s="81" t="str">
         <f>'SBH-FORM 1'!D5</f>
         <v>Contractor</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="12"/>
-      <c r="J4" s="101" t="s">
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="11"/>
+      <c r="J4" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="87"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="85">
+      <c r="K4" s="83"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="81">
         <f>'SBH-FORM 1'!G5</f>
         <v>0</v>
       </c>
-      <c r="N4" s="86"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="1:26" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="86"/>
-      <c r="O5" s="110"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="36"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="33"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="85" t="str">
+      <c r="C6" s="81" t="str">
         <f>'SBH-FORM 1'!D7</f>
         <v>Period</v>
       </c>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="J6" s="101" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" s="87"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="85">
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="J6" s="97" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="83"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="81">
         <f>'SBH-FORM 1'!G7</f>
         <v>0</v>
       </c>
-      <c r="N6" s="109"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="36"/>
+      <c r="N6" s="105"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="33"/>
     </row>
     <row r="7" spans="1:26" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="36"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="104"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="33"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="170"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="171"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="112"/>
-      <c r="O8" s="113"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="36"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="173"/>
+      <c r="D8" s="173"/>
+      <c r="E8" s="173"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="174"/>
+      <c r="J8" s="174"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="108"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="33"/>
     </row>
     <row r="9" spans="1:26" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="36"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="33"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="172" t="str">
+      <c r="B11" s="175" t="str">
         <f>'SBH-FORM 1'!B10</f>
         <v xml:space="preserve">Outsource Service Description : </v>
       </c>
-      <c r="C11" s="173"/>
-      <c r="D11" s="173"/>
-      <c r="E11" s="173"/>
-      <c r="F11" s="173"/>
-      <c r="G11" s="173"/>
-      <c r="H11" s="173"/>
-      <c r="I11" s="173" t="str">
+      <c r="C11" s="176"/>
+      <c r="D11" s="176"/>
+      <c r="E11" s="176"/>
+      <c r="F11" s="176"/>
+      <c r="G11" s="176"/>
+      <c r="H11" s="176"/>
+      <c r="I11" s="176" t="str">
         <f>'SBH-FORM 1'!J10</f>
         <v>Team Based Hiring for Division Name</v>
       </c>
-      <c r="J11" s="173"/>
-      <c r="K11" s="173"/>
-      <c r="L11" s="173"/>
-      <c r="M11" s="173"/>
-      <c r="N11" s="174"/>
-      <c r="O11" s="174"/>
-      <c r="P11" s="175"/>
-      <c r="Q11" s="36"/>
+      <c r="J11" s="176"/>
+      <c r="K11" s="176"/>
+      <c r="L11" s="176"/>
+      <c r="M11" s="176"/>
+      <c r="N11" s="177"/>
+      <c r="O11" s="177"/>
+      <c r="P11" s="178"/>
+      <c r="Q11" s="33"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="168"/>
-      <c r="C12" s="169"/>
-      <c r="D12" s="169"/>
-      <c r="E12" s="169"/>
-      <c r="F12" s="169"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="169"/>
-      <c r="I12" s="169"/>
-      <c r="J12" s="169"/>
-      <c r="K12" s="169"/>
-      <c r="L12" s="169"/>
-      <c r="M12" s="169"/>
-      <c r="N12" s="176"/>
-      <c r="O12" s="176"/>
-      <c r="P12" s="141"/>
-      <c r="Q12" s="36"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="172"/>
+      <c r="D12" s="172"/>
+      <c r="E12" s="172"/>
+      <c r="F12" s="172"/>
+      <c r="G12" s="172"/>
+      <c r="H12" s="172"/>
+      <c r="I12" s="172"/>
+      <c r="J12" s="172"/>
+      <c r="K12" s="172"/>
+      <c r="L12" s="172"/>
+      <c r="M12" s="172"/>
+      <c r="N12" s="179"/>
+      <c r="O12" s="179"/>
+      <c r="P12" s="142"/>
+      <c r="Q12" s="33"/>
     </row>
     <row r="13" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="168" t="s">
+      <c r="B13" s="171" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="169" t="s">
+      <c r="C13" s="172" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="169" t="s">
+      <c r="D13" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="169"/>
-      <c r="F13" s="169"/>
-      <c r="G13" s="169" t="s">
+      <c r="E13" s="172"/>
+      <c r="F13" s="172"/>
+      <c r="G13" s="172" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="169"/>
-      <c r="I13" s="169"/>
-      <c r="J13" s="169" t="s">
+      <c r="H13" s="172"/>
+      <c r="I13" s="172"/>
+      <c r="J13" s="172" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="169"/>
-      <c r="L13" s="169"/>
-      <c r="M13" s="140" t="s">
+      <c r="K13" s="172"/>
+      <c r="L13" s="172"/>
+      <c r="M13" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="N13" s="140" t="s">
+      <c r="N13" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="O13" s="140" t="s">
+      <c r="O13" s="141" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="141" t="s">
+      <c r="P13" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="137">
+      <c r="Q13" s="33"/>
+      <c r="R13" s="138">
         <v>180</v>
       </c>
-      <c r="S13" s="138"/>
-      <c r="T13" s="139"/>
+      <c r="S13" s="139"/>
+      <c r="T13" s="140"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="168"/>
-      <c r="C14" s="169"/>
-      <c r="D14" s="96" t="s">
+      <c r="B14" s="171"/>
+      <c r="C14" s="172"/>
+      <c r="D14" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="96" t="s">
+      <c r="E14" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="96" t="s">
+      <c r="F14" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="96" t="s">
+      <c r="G14" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="96" t="s">
+      <c r="H14" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="96" t="s">
+      <c r="I14" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="96" t="s">
+      <c r="J14" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="96" t="s">
+      <c r="K14" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="L14" s="96" t="s">
+      <c r="L14" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="M14" s="140"/>
-      <c r="N14" s="140"/>
-      <c r="O14" s="140"/>
-      <c r="P14" s="141"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="37" t="s">
+      <c r="M14" s="141"/>
+      <c r="N14" s="141"/>
+      <c r="O14" s="141"/>
+      <c r="P14" s="142"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="38" t="s">
+      <c r="S14" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="T14" s="71" t="s">
+      <c r="T14" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="U14" s="81" t="str">
+      <c r="U14" s="77" t="str">
         <f t="shared" ref="U14:U17" si="0">CONCATENATE(B14," ",C14," ",N14)</f>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="Z14" s="81" t="s">
+      <c r="Z14" s="77" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="53"/>
-      <c r="C15" s="88"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="97"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="72"/>
-      <c r="U15" s="81" t="str">
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="71"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="68"/>
+      <c r="U15" s="77" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="Z15" s="81" t="s">
+      <c r="Z15" s="77" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58">
+      <c r="A16" s="50"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54">
         <f t="shared" ref="G16" si="1">R16/$R$13</f>
         <v>0</v>
       </c>
-      <c r="H16" s="58">
+      <c r="H16" s="54">
         <f t="shared" ref="H16" si="2">S16/$R$13</f>
         <v>0</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I16" s="54">
         <f t="shared" ref="I16" si="3">T16/$R$13</f>
         <v>0</v>
       </c>
-      <c r="J16" s="62" t="e">
+      <c r="J16" s="58" t="e">
         <f>VLOOKUP($C16,'UNIT PRICE'!$A:$E,2,TRUE)</f>
         <v>#N/A</v>
       </c>
-      <c r="K16" s="62" t="e">
+      <c r="K16" s="58" t="e">
         <f>VLOOKUP($C16,'UNIT PRICE'!$A:$E,3,TRUE)</f>
         <v>#N/A</v>
       </c>
-      <c r="L16" s="62" t="e">
+      <c r="L16" s="58" t="e">
         <f>VLOOKUP($C16,'UNIT PRICE'!$A:$E,4,TRUE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M16" s="63" t="e">
+      <c r="M16" s="59" t="e">
         <f t="shared" ref="M16" si="4">(G16*J16) + (H16*K16) + (I16*L16)</f>
         <v>#N/A</v>
       </c>
-      <c r="N16" s="76"/>
-      <c r="O16" s="76" t="e">
+      <c r="N16" s="72"/>
+      <c r="O16" s="72" t="e">
         <f t="shared" ref="O16" si="5">M16+N16*M16</f>
         <v>#N/A</v>
       </c>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="59"/>
-      <c r="R16" s="65">
+      <c r="P16" s="60"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="61">
         <f>SUMIFS('SBH-FORM 1'!$S:$S,'SBH-FORM 1'!$Q:$Q,$U16,'SBH-FORM 1'!$R:$R,R$14)</f>
         <v>0</v>
       </c>
-      <c r="S16" s="65">
+      <c r="S16" s="61">
         <f>SUMIFS('SBH-FORM 1'!$S:$S,'SBH-FORM 1'!$Q:$Q,$U16,'SBH-FORM 1'!$R:$R,S$14)</f>
         <v>0</v>
       </c>
-      <c r="T16" s="73">
+      <c r="T16" s="69">
         <f>SUMIFS('SBH-FORM 1'!$S:$S,'SBH-FORM 1'!$Q:$Q,$U16,'SBH-FORM 1'!$R:$R,T$14)</f>
         <v>0</v>
       </c>
-      <c r="U16" s="81" t="str">
+      <c r="U16" s="77" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="Z16" s="81" t="s">
+      <c r="Z16" s="77" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:26" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="51"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="77"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="74"/>
-      <c r="U17" s="81" t="str">
+      <c r="B17" s="47"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="70"/>
+      <c r="U17" s="77" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  </v>
       </c>
-      <c r="Z17" s="81" t="s">
+      <c r="Z17" s="77" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B18" s="142"/>
-      <c r="C18" s="143"/>
-      <c r="D18" s="143"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
-      <c r="K18" s="143"/>
-      <c r="L18" s="144"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="77" t="s">
+      <c r="B18" s="143"/>
+      <c r="C18" s="144"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="144"/>
+      <c r="F18" s="144"/>
+      <c r="G18" s="144"/>
+      <c r="H18" s="144"/>
+      <c r="I18" s="144"/>
+      <c r="J18" s="144"/>
+      <c r="K18" s="144"/>
+      <c r="L18" s="145"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="O18" s="48" t="e">
+      <c r="O18" s="44" t="e">
         <f ca="1">SUM(O16:INDIRECT("O"&amp;ROW()-2))</f>
         <v>#N/A</v>
       </c>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="36"/>
-      <c r="Z18" s="81" t="s">
+      <c r="P18" s="26"/>
+      <c r="Q18" s="33"/>
+      <c r="Z18" s="77" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="152"/>
-      <c r="D19" s="154"/>
-      <c r="E19" s="154"/>
-      <c r="F19" s="154"/>
-      <c r="G19" s="155">
+      <c r="C19" s="153"/>
+      <c r="D19" s="157"/>
+      <c r="E19" s="157"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="158">
         <f>COUNTIF('SBH-FORM 1'!T:T, "YES")</f>
         <v>0</v>
       </c>
-      <c r="H19" s="155"/>
-      <c r="I19" s="155"/>
-      <c r="J19" s="156">
+      <c r="H19" s="158"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="159">
         <v>160</v>
       </c>
-      <c r="K19" s="156"/>
-      <c r="L19" s="156"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="84">
+      <c r="K19" s="159"/>
+      <c r="L19" s="159"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="80">
         <f>G19*J19</f>
         <v>0</v>
       </c>
       <c r="P19" s="2"/>
-      <c r="Q19" s="36"/>
-      <c r="Z19" s="81" t="s">
+      <c r="Q19" s="33"/>
+      <c r="Z19" s="77" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:26" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="18"/>
-      <c r="M20" s="145" t="s">
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="15"/>
+      <c r="M20" s="146" t="s">
         <v>50</v>
       </c>
-      <c r="N20" s="146"/>
-      <c r="O20" s="107" t="e">
+      <c r="N20" s="147"/>
+      <c r="O20" s="103" t="e">
         <f ca="1">INDIRECT("O"&amp;ROW()-2)-INDIRECT("O"&amp;ROW()-1)</f>
         <v>#N/A</v>
       </c>
-      <c r="Q20" s="36"/>
+      <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="147" t="s">
+      <c r="B21" s="148" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="147"/>
-      <c r="D21" s="147"/>
-      <c r="E21" s="147"/>
-      <c r="F21" s="147"/>
-      <c r="G21" s="147"/>
-      <c r="H21" s="147"/>
-      <c r="I21" s="147"/>
-      <c r="J21" s="147"/>
-      <c r="K21" s="147"/>
-      <c r="L21" s="147"/>
-      <c r="M21" s="147"/>
-      <c r="N21" s="147"/>
-      <c r="O21" s="147"/>
-      <c r="P21" s="147"/>
-      <c r="Q21" s="36"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="148"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
+      <c r="H21" s="148"/>
+      <c r="I21" s="148"/>
+      <c r="J21" s="148"/>
+      <c r="K21" s="148"/>
+      <c r="L21" s="148"/>
+      <c r="M21" s="148"/>
+      <c r="N21" s="148"/>
+      <c r="O21" s="148"/>
+      <c r="P21" s="148"/>
+      <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
     </row>
     <row r="23" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="36"/>
-      <c r="C23" s="148" t="s">
+      <c r="B23" s="33"/>
+      <c r="C23" s="149" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="149"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="92" t="s">
+      <c r="D23" s="150"/>
+      <c r="E23" s="150"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="17"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="42" t="s">
+      <c r="J23" s="111"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="111"/>
+      <c r="M23" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
     </row>
     <row r="24" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="36"/>
-      <c r="C24" s="149"/>
-      <c r="D24" s="149"/>
-      <c r="E24" s="149"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="150"/>
+      <c r="D24" s="150"/>
+      <c r="E24" s="150"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
     </row>
     <row r="25" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="36"/>
-      <c r="C25" s="149"/>
-      <c r="D25" s="149"/>
-      <c r="E25" s="149"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="92" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="42" t="s">
+      <c r="J25" s="111"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="111"/>
+      <c r="M25" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="36"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
     </row>
     <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="36"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
     </row>
     <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="91"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="150" t="s">
+      <c r="B27" s="87"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="H27" s="150"/>
-      <c r="I27" s="150"/>
-      <c r="J27" s="153"/>
-      <c r="K27" s="138"/>
-      <c r="L27" s="139"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="36"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="154"/>
+      <c r="K27" s="155"/>
+      <c r="L27" s="156"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
     </row>
     <row r="28" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="91"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="92"/>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
+      <c r="B28" s="87"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="88"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
     </row>
     <row r="29" spans="2:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="91"/>
-      <c r="C29" s="157" t="s">
+      <c r="B29" s="87"/>
+      <c r="C29" s="160" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="157"/>
-      <c r="E29" s="157"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="158" t="s">
+      <c r="D29" s="160"/>
+      <c r="E29" s="160"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="161" t="s">
         <v>59</v>
       </c>
-      <c r="H29" s="158"/>
-      <c r="I29" s="158"/>
-      <c r="J29" s="159" t="s">
+      <c r="H29" s="161"/>
+      <c r="I29" s="161"/>
+      <c r="J29" s="162" t="s">
         <v>60</v>
       </c>
-      <c r="K29" s="160"/>
-      <c r="L29" s="13" t="s">
+      <c r="K29" s="163"/>
+      <c r="L29" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="M29" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="N29" s="79"/>
-      <c r="O29" s="79"/>
-      <c r="P29" s="36"/>
-      <c r="Q29" s="36"/>
+      <c r="M29" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="N29" s="75"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
     </row>
     <row r="30" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="91"/>
-      <c r="C30" s="157"/>
-      <c r="D30" s="157"/>
-      <c r="E30" s="157"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="161"/>
-      <c r="H30" s="162"/>
-      <c r="I30" s="163"/>
-      <c r="J30" s="164"/>
-      <c r="K30" s="165"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="80"/>
-      <c r="O30" s="80"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="160"/>
+      <c r="D30" s="160"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="164"/>
+      <c r="H30" s="165"/>
+      <c r="I30" s="166"/>
+      <c r="J30" s="167"/>
+      <c r="K30" s="168"/>
+      <c r="L30" s="112"/>
+      <c r="M30" s="113"/>
+      <c r="N30" s="76"/>
+      <c r="O30" s="76"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C32" s="94" t="s">
+      <c r="C32" s="90" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="169" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="166" t="s">
+      <c r="E32" s="169"/>
+      <c r="F32" s="169"/>
+      <c r="G32" s="169"/>
+      <c r="H32" s="169"/>
+      <c r="I32" s="169"/>
+      <c r="J32" s="169"/>
+      <c r="K32" s="169"/>
+      <c r="L32" s="169"/>
+      <c r="M32" s="169"/>
+      <c r="N32" s="169"/>
+      <c r="O32" s="169"/>
+      <c r="P32" s="169"/>
+    </row>
+    <row r="33" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C33" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="166"/>
-      <c r="F32" s="166"/>
-      <c r="G32" s="166"/>
-      <c r="H32" s="166"/>
-      <c r="I32" s="166"/>
-      <c r="J32" s="166"/>
-      <c r="K32" s="166"/>
-      <c r="L32" s="166"/>
-      <c r="M32" s="166"/>
-      <c r="N32" s="166"/>
-      <c r="O32" s="166"/>
-      <c r="P32" s="166"/>
-    </row>
-    <row r="33" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C33" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="167"/>
-      <c r="E33" s="167"/>
-      <c r="F33" s="167"/>
-      <c r="G33" s="167"/>
-      <c r="H33" s="167"/>
-      <c r="I33" s="167"/>
-      <c r="J33" s="167"/>
-      <c r="K33" s="167"/>
-      <c r="L33" s="167"/>
-      <c r="M33" s="167"/>
-      <c r="N33" s="167"/>
-      <c r="O33" s="167"/>
-      <c r="P33" s="167"/>
+      <c r="D33" s="170"/>
+      <c r="E33" s="170"/>
+      <c r="F33" s="170"/>
+      <c r="G33" s="170"/>
+      <c r="H33" s="170"/>
+      <c r="I33" s="170"/>
+      <c r="J33" s="170"/>
+      <c r="K33" s="170"/>
+      <c r="L33" s="170"/>
+      <c r="M33" s="170"/>
+      <c r="N33" s="170"/>
+      <c r="O33" s="170"/>
+      <c r="P33" s="170"/>
     </row>
     <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
     </row>
     <row r="36" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="114" t="s">
+      <c r="C36" s="115" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="115"/>
+      <c r="E36" s="115"/>
+      <c r="F36" s="115"/>
+      <c r="G36" s="115"/>
+      <c r="M36" s="77"/>
+      <c r="N36" s="115" t="s">
+        <v>77</v>
+      </c>
+      <c r="O36" s="115"/>
+      <c r="P36" s="115"/>
+      <c r="Q36" s="98"/>
+      <c r="R36" s="101"/>
+    </row>
+    <row r="37" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="137" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="137"/>
+      <c r="E37" s="137"/>
+      <c r="F37" s="137"/>
+      <c r="G37" s="137"/>
+      <c r="M37" s="77"/>
+      <c r="N37" s="117" t="s">
+        <v>76</v>
+      </c>
+      <c r="O37" s="117"/>
+      <c r="P37" s="117"/>
+      <c r="Q37" s="99"/>
+      <c r="R37" s="101"/>
+    </row>
+    <row r="38" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="114"/>
-      <c r="E36" s="114"/>
-      <c r="F36" s="114"/>
-      <c r="G36" s="114"/>
-      <c r="M36" s="81"/>
-      <c r="N36" s="114" t="s">
-        <v>78</v>
-      </c>
-      <c r="O36" s="114"/>
-      <c r="P36" s="114"/>
-      <c r="Q36" s="102"/>
-      <c r="R36" s="105"/>
-    </row>
-    <row r="37" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="136" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="136"/>
-      <c r="F37" s="136"/>
-      <c r="G37" s="136"/>
-      <c r="M37" s="81"/>
-      <c r="N37" s="115" t="s">
-        <v>77</v>
-      </c>
-      <c r="O37" s="115"/>
-      <c r="P37" s="115"/>
-      <c r="Q37" s="103"/>
-      <c r="R37" s="105"/>
-    </row>
-    <row r="38" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="135" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="135"/>
-      <c r="E38" s="135"/>
-      <c r="F38" s="135"/>
-      <c r="G38" s="135"/>
-      <c r="M38" s="81"/>
-      <c r="N38" s="135" t="s">
-        <v>67</v>
-      </c>
-      <c r="O38" s="135"/>
-      <c r="P38" s="135"/>
-      <c r="Q38" s="104"/>
-      <c r="R38" s="105"/>
+      <c r="D38" s="136"/>
+      <c r="E38" s="136"/>
+      <c r="F38" s="136"/>
+      <c r="G38" s="136"/>
+      <c r="M38" s="77"/>
+      <c r="N38" s="136" t="s">
+        <v>66</v>
+      </c>
+      <c r="O38" s="136"/>
+      <c r="P38" s="136"/>
+      <c r="Q38" s="100"/>
+      <c r="R38" s="101"/>
     </row>
     <row r="39" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="135" t="s">
+      <c r="C39" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="135"/>
-      <c r="E39" s="135"/>
-      <c r="F39" s="135"/>
-      <c r="G39" s="135"/>
-      <c r="M39" s="81"/>
-      <c r="N39" s="135" t="s">
+      <c r="D39" s="136"/>
+      <c r="E39" s="136"/>
+      <c r="F39" s="136"/>
+      <c r="G39" s="136"/>
+      <c r="M39" s="77"/>
+      <c r="N39" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="O39" s="135"/>
-      <c r="P39" s="135"/>
-      <c r="Q39" s="104"/>
-      <c r="R39" s="105"/>
+      <c r="O39" s="136"/>
+      <c r="P39" s="136"/>
+      <c r="Q39" s="100"/>
+      <c r="R39" s="101"/>
     </row>
     <row r="40" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="115" t="s">
+      <c r="C40" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115"/>
-      <c r="F40" s="115"/>
-      <c r="G40" s="115"/>
-      <c r="M40" s="81"/>
-      <c r="N40" s="115" t="s">
+      <c r="D40" s="117"/>
+      <c r="E40" s="117"/>
+      <c r="F40" s="117"/>
+      <c r="G40" s="117"/>
+      <c r="M40" s="77"/>
+      <c r="N40" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="O40" s="115"/>
-      <c r="P40" s="115"/>
-      <c r="Q40" s="103"/>
-      <c r="R40" s="105"/>
+      <c r="O40" s="117"/>
+      <c r="P40" s="117"/>
+      <c r="Q40" s="99"/>
+      <c r="R40" s="101"/>
     </row>
     <row r="42" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="N42" s="81"/>
-      <c r="O42" s="81"/>
+      <c r="N42" s="77"/>
+      <c r="O42" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -3435,7 +3457,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>3000</v>
@@ -3452,7 +3474,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3">
         <v>4500</v>
@@ -3503,7 +3525,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6">
         <v>5379</v>
@@ -3537,7 +3559,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8">
         <v>3000</v>

</xml_diff>

<commit_message>
Fix SBH to show proper total required hours
</commit_message>
<xml_diff>
--- a/creator/forms_xlsx/SBH-FORM.xlsx
+++ b/creator/forms_xlsx/SBH-FORM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo_dev\extra_addons\budget_outsource\creator\forms_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo_dev\_extra_addons\budget_outsource\creator\forms_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="SBH-FORM 1" sheetId="1" r:id="rId1"/>
@@ -905,7 +905,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1221,6 +1221,60 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1231,59 +1285,140 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1293,140 +1428,39 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1715,8 +1749,8 @@
   </sheetPr>
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1763,8 @@
     <col min="7" max="7" width="9.5703125" style="77" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" style="77" customWidth="1"/>
     <col min="9" max="9" width="10" style="77" customWidth="1"/>
-    <col min="10" max="11" width="12.7109375" style="77" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="180" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="77" customWidth="1"/>
     <col min="12" max="12" width="17.140625" style="77" customWidth="1"/>
     <col min="13" max="14" width="26.42578125" style="77" customWidth="1"/>
     <col min="15" max="15" width="22.28515625" style="77" customWidth="1"/>
@@ -1744,41 +1779,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="118" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="118"/>
+      <c r="B1" s="115" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
       <c r="P1" s="33"/>
     </row>
     <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
       <c r="P2" s="33"/>
     </row>
     <row r="3" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1796,7 +1831,7 @@
       <c r="G4" s="94"/>
       <c r="H4" s="94"/>
       <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
+      <c r="J4" s="181"/>
       <c r="K4" s="94"/>
       <c r="L4" s="94"/>
       <c r="M4" s="94"/>
@@ -1881,7 +1916,7 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
+      <c r="J8" s="182"/>
       <c r="K8" s="28"/>
       <c r="L8" s="45"/>
       <c r="M8" s="45"/>
@@ -1901,7 +1936,7 @@
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="J9" s="183"/>
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
       <c r="M9" s="33"/>
@@ -1913,65 +1948,65 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="127" t="s">
+      <c r="B10" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="128"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
-      <c r="I10" s="129"/>
-      <c r="J10" s="121" t="s">
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="126"/>
+      <c r="J10" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="K10" s="121"/>
-      <c r="L10" s="121"/>
-      <c r="M10" s="121"/>
-      <c r="N10" s="121"/>
-      <c r="O10" s="121"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="118"/>
+      <c r="M10" s="118"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="118"/>
       <c r="P10" s="33"/>
       <c r="Y10" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="130"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="131"/>
-      <c r="I11" s="132"/>
-      <c r="J11" s="122"/>
-      <c r="K11" s="122"/>
-      <c r="L11" s="122"/>
-      <c r="M11" s="122"/>
-      <c r="N11" s="122"/>
-      <c r="O11" s="122"/>
+      <c r="B11" s="127"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="129"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="119"/>
+      <c r="O11" s="119"/>
       <c r="P11" s="33"/>
       <c r="Y11" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="134"/>
-      <c r="H12" s="134"/>
-      <c r="I12" s="134"/>
-      <c r="J12" s="134"/>
-      <c r="K12" s="134"/>
-      <c r="L12" s="134"/>
-      <c r="M12" s="134"/>
-      <c r="N12" s="135"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="131"/>
+      <c r="G12" s="131"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="131"/>
+      <c r="J12" s="131"/>
+      <c r="K12" s="131"/>
+      <c r="L12" s="131"/>
+      <c r="M12" s="131"/>
+      <c r="N12" s="132"/>
       <c r="O12" s="29" t="s">
         <v>5</v>
       </c>
@@ -2005,7 +2040,7 @@
       <c r="I13" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J13" s="92" t="s">
+      <c r="J13" s="184" t="s">
         <v>15</v>
       </c>
       <c r="K13" s="92" t="s">
@@ -2051,7 +2086,7 @@
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
       <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
+      <c r="J14" s="185"/>
       <c r="K14" s="65"/>
       <c r="L14" s="65"/>
       <c r="M14" s="66"/>
@@ -2103,7 +2138,7 @@
       <c r="I15" s="65">
         <v>7</v>
       </c>
-      <c r="J15" s="65">
+      <c r="J15" s="185">
         <v>8</v>
       </c>
       <c r="K15" s="110">
@@ -2183,14 +2218,14 @@
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="123" t="s">
+      <c r="E17" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="124"/>
+      <c r="F17" s="121"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="J17" s="186"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -2226,7 +2261,7 @@
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
       <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
+      <c r="J18" s="187"/>
       <c r="K18" s="43"/>
       <c r="L18" s="43"/>
       <c r="M18" s="43"/>
@@ -2262,7 +2297,7 @@
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
       <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="J19" s="187"/>
       <c r="K19" s="43"/>
       <c r="L19" s="43"/>
       <c r="M19" s="43"/>
@@ -2298,7 +2333,7 @@
       <c r="G20" s="89"/>
       <c r="H20" s="89"/>
       <c r="I20" s="89"/>
-      <c r="J20" s="89"/>
+      <c r="J20" s="188"/>
       <c r="K20" s="89"/>
       <c r="L20" s="89"/>
       <c r="M20" s="89"/>
@@ -2334,7 +2369,7 @@
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
+      <c r="J21" s="189"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
@@ -2346,16 +2381,16 @@
       </c>
     </row>
     <row r="22" spans="1:25" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="125"/>
-      <c r="B22" s="126"/>
-      <c r="C22" s="126"/>
-      <c r="D22" s="126"/>
-      <c r="E22" s="126"/>
+      <c r="A22" s="122"/>
+      <c r="B22" s="123"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
       <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="J22" s="183"/>
       <c r="K22" s="33"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -2373,24 +2408,24 @@
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="115" t="s">
+      <c r="B24" s="133" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="115"/>
-      <c r="D24" s="115"/>
-      <c r="E24" s="115"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
       <c r="L24" s="101"/>
       <c r="M24" s="98"/>
       <c r="N24" s="98"/>
       <c r="O24" s="98"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B25" s="116" t="s">
+      <c r="B25" s="134" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="116"/>
-      <c r="D25" s="116"/>
-      <c r="E25" s="116"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
       <c r="L25" s="101"/>
       <c r="M25" s="100"/>
       <c r="N25" s="100"/>
@@ -2400,12 +2435,13 @@
       </c>
     </row>
     <row r="26" spans="1:25" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="117" t="s">
+      <c r="B26" s="135" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="117"/>
-      <c r="D26" s="117"/>
-      <c r="E26" s="117"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="135"/>
+      <c r="J26" s="190"/>
       <c r="L26" s="96"/>
       <c r="M26" s="99"/>
       <c r="N26" s="99"/>
@@ -2413,12 +2449,13 @@
       <c r="T26" s="102"/>
     </row>
     <row r="27" spans="1:25" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="117"/>
-      <c r="D27" s="117"/>
-      <c r="E27" s="117"/>
+      <c r="C27" s="135"/>
+      <c r="D27" s="135"/>
+      <c r="E27" s="135"/>
+      <c r="J27" s="190"/>
       <c r="L27" s="96"/>
       <c r="M27" s="99"/>
       <c r="N27" s="99"/>
@@ -2426,12 +2463,13 @@
       <c r="T27" s="102"/>
     </row>
     <row r="28" spans="1:25" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
-      <c r="E28" s="117"/>
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="135"/>
+      <c r="J28" s="190"/>
       <c r="L28" s="96"/>
       <c r="M28" s="99"/>
       <c r="N28" s="99"/>
@@ -2454,10 +2492,15 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
+      <c r="J34" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="J10:O11"/>
@@ -2465,11 +2508,6 @@
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="B10:I11"/>
     <mergeCell ref="B12:N12"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2487,8 +2525,8 @@
   </sheetPr>
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,23 +2550,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="118"/>
-      <c r="P1" s="118"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
       <c r="Q1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2550,23 +2588,23 @@
       <c r="Q2" s="33"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="148" t="s">
+      <c r="B3" s="138" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="148"/>
-      <c r="N3" s="148"/>
-      <c r="O3" s="148"/>
-      <c r="P3" s="148"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="138"/>
+      <c r="O3" s="138"/>
+      <c r="P3" s="138"/>
       <c r="Q3" s="33"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2658,14 +2696,14 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11"/>
-      <c r="C8" s="173"/>
-      <c r="D8" s="173"/>
-      <c r="E8" s="173"/>
-      <c r="F8" s="174"/>
-      <c r="G8" s="174"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="141"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="142"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="174"/>
-      <c r="J8" s="174"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="142"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="37"/>
@@ -2711,91 +2749,91 @@
       <c r="Q10" s="33"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="175" t="str">
+      <c r="B11" s="143" t="str">
         <f>'SBH-FORM 1'!B10</f>
         <v xml:space="preserve">Outsource Service Description : </v>
       </c>
-      <c r="C11" s="176"/>
-      <c r="D11" s="176"/>
-      <c r="E11" s="176"/>
-      <c r="F11" s="176"/>
-      <c r="G11" s="176"/>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176" t="str">
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
+      <c r="F11" s="144"/>
+      <c r="G11" s="144"/>
+      <c r="H11" s="144"/>
+      <c r="I11" s="144" t="str">
         <f>'SBH-FORM 1'!J10</f>
         <v>Team Based Hiring for Division Name</v>
       </c>
-      <c r="J11" s="176"/>
-      <c r="K11" s="176"/>
-      <c r="L11" s="176"/>
-      <c r="M11" s="176"/>
-      <c r="N11" s="177"/>
-      <c r="O11" s="177"/>
-      <c r="P11" s="178"/>
+      <c r="J11" s="144"/>
+      <c r="K11" s="144"/>
+      <c r="L11" s="144"/>
+      <c r="M11" s="144"/>
+      <c r="N11" s="145"/>
+      <c r="O11" s="145"/>
+      <c r="P11" s="146"/>
       <c r="Q11" s="33"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="171"/>
-      <c r="C12" s="172"/>
-      <c r="D12" s="172"/>
-      <c r="E12" s="172"/>
-      <c r="F12" s="172"/>
-      <c r="G12" s="172"/>
-      <c r="H12" s="172"/>
-      <c r="I12" s="172"/>
-      <c r="J12" s="172"/>
-      <c r="K12" s="172"/>
-      <c r="L12" s="172"/>
-      <c r="M12" s="172"/>
-      <c r="N12" s="179"/>
-      <c r="O12" s="179"/>
-      <c r="P12" s="142"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="140"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="140"/>
+      <c r="I12" s="140"/>
+      <c r="J12" s="140"/>
+      <c r="K12" s="140"/>
+      <c r="L12" s="140"/>
+      <c r="M12" s="140"/>
+      <c r="N12" s="147"/>
+      <c r="O12" s="147"/>
+      <c r="P12" s="148"/>
       <c r="Q12" s="33"/>
     </row>
     <row r="13" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="172" t="s">
+      <c r="C13" s="140" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="172" t="s">
+      <c r="D13" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="172"/>
-      <c r="F13" s="172"/>
-      <c r="G13" s="172" t="s">
+      <c r="E13" s="140"/>
+      <c r="F13" s="140"/>
+      <c r="G13" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="172"/>
-      <c r="I13" s="172"/>
-      <c r="J13" s="172" t="s">
+      <c r="H13" s="140"/>
+      <c r="I13" s="140"/>
+      <c r="J13" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="172"/>
-      <c r="L13" s="172"/>
-      <c r="M13" s="141" t="s">
+      <c r="K13" s="140"/>
+      <c r="L13" s="140"/>
+      <c r="M13" s="149" t="s">
         <v>43</v>
       </c>
-      <c r="N13" s="141" t="s">
+      <c r="N13" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="O13" s="141" t="s">
+      <c r="O13" s="149" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="142" t="s">
+      <c r="P13" s="148" t="s">
         <v>18</v>
       </c>
       <c r="Q13" s="33"/>
-      <c r="R13" s="138">
+      <c r="R13" s="172">
         <v>180</v>
       </c>
-      <c r="S13" s="139"/>
-      <c r="T13" s="140"/>
+      <c r="S13" s="173"/>
+      <c r="T13" s="174"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="171"/>
-      <c r="C14" s="172"/>
+      <c r="B14" s="139"/>
+      <c r="C14" s="140"/>
       <c r="D14" s="92" t="s">
         <v>45</v>
       </c>
@@ -2823,10 +2861,10 @@
       <c r="L14" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="M14" s="141"/>
-      <c r="N14" s="141"/>
-      <c r="O14" s="141"/>
-      <c r="P14" s="142"/>
+      <c r="M14" s="149"/>
+      <c r="N14" s="149"/>
+      <c r="O14" s="149"/>
+      <c r="P14" s="148"/>
       <c r="Q14" s="33"/>
       <c r="R14" s="34" t="s">
         <v>22</v>
@@ -2964,17 +3002,17 @@
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B18" s="143"/>
-      <c r="C18" s="144"/>
-      <c r="D18" s="144"/>
-      <c r="E18" s="144"/>
-      <c r="F18" s="144"/>
-      <c r="G18" s="144"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="144"/>
-      <c r="J18" s="144"/>
-      <c r="K18" s="144"/>
-      <c r="L18" s="145"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="176"/>
+      <c r="D18" s="176"/>
+      <c r="E18" s="176"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="176"/>
+      <c r="H18" s="176"/>
+      <c r="I18" s="176"/>
+      <c r="J18" s="176"/>
+      <c r="K18" s="176"/>
+      <c r="L18" s="177"/>
       <c r="M18" s="44"/>
       <c r="N18" s="73" t="s">
         <v>48</v>
@@ -2990,24 +3028,24 @@
       </c>
     </row>
     <row r="19" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="152" t="s">
+      <c r="B19" s="164" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="153"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="158">
+      <c r="C19" s="165"/>
+      <c r="D19" s="169"/>
+      <c r="E19" s="169"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="170">
         <f>COUNTIF('SBH-FORM 1'!T:T, "YES")</f>
         <v>0</v>
       </c>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="159">
+      <c r="H19" s="170"/>
+      <c r="I19" s="170"/>
+      <c r="J19" s="171">
         <v>160</v>
       </c>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
+      <c r="K19" s="171"/>
+      <c r="L19" s="171"/>
       <c r="M19" s="48"/>
       <c r="N19" s="74"/>
       <c r="O19" s="80">
@@ -3030,10 +3068,10 @@
       <c r="H20" s="33"/>
       <c r="I20" s="33"/>
       <c r="J20" s="15"/>
-      <c r="M20" s="146" t="s">
+      <c r="M20" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="N20" s="147"/>
+      <c r="N20" s="160"/>
       <c r="O20" s="103" t="e">
         <f ca="1">INDIRECT("O"&amp;ROW()-2)-INDIRECT("O"&amp;ROW()-1)</f>
         <v>#N/A</v>
@@ -3041,23 +3079,23 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="148" t="s">
+      <c r="B21" s="138" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
-      <c r="H21" s="148"/>
-      <c r="I21" s="148"/>
-      <c r="J21" s="148"/>
-      <c r="K21" s="148"/>
-      <c r="L21" s="148"/>
-      <c r="M21" s="148"/>
-      <c r="N21" s="148"/>
-      <c r="O21" s="148"/>
-      <c r="P21" s="148"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138"/>
+      <c r="E21" s="138"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="138"/>
+      <c r="I21" s="138"/>
+      <c r="J21" s="138"/>
+      <c r="K21" s="138"/>
+      <c r="L21" s="138"/>
+      <c r="M21" s="138"/>
+      <c r="N21" s="138"/>
+      <c r="O21" s="138"/>
+      <c r="P21" s="138"/>
       <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3080,11 +3118,11 @@
     </row>
     <row r="23" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
-      <c r="C23" s="149" t="s">
+      <c r="C23" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="150"/>
-      <c r="E23" s="150"/>
+      <c r="D23" s="162"/>
+      <c r="E23" s="162"/>
       <c r="F23" s="33"/>
       <c r="G23" s="33"/>
       <c r="H23" s="33"/>
@@ -3104,9 +3142,9 @@
     </row>
     <row r="24" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
-      <c r="C24" s="150"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="150"/>
+      <c r="C24" s="162"/>
+      <c r="D24" s="162"/>
+      <c r="E24" s="162"/>
       <c r="F24" s="33"/>
       <c r="G24" s="33"/>
       <c r="H24" s="33"/>
@@ -3122,9 +3160,9 @@
     </row>
     <row r="25" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="33"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="150"/>
+      <c r="C25" s="162"/>
+      <c r="D25" s="162"/>
+      <c r="E25" s="162"/>
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
       <c r="H25" s="33"/>
@@ -3163,14 +3201,14 @@
     <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="87"/>
       <c r="F27" s="33"/>
-      <c r="G27" s="151" t="s">
+      <c r="G27" s="163" t="s">
         <v>57</v>
       </c>
-      <c r="H27" s="151"/>
-      <c r="I27" s="151"/>
-      <c r="J27" s="154"/>
-      <c r="K27" s="155"/>
-      <c r="L27" s="156"/>
+      <c r="H27" s="163"/>
+      <c r="I27" s="163"/>
+      <c r="J27" s="166"/>
+      <c r="K27" s="167"/>
+      <c r="L27" s="168"/>
       <c r="M27" s="38"/>
       <c r="N27" s="38"/>
       <c r="O27" s="38"/>
@@ -3194,21 +3232,21 @@
     </row>
     <row r="29" spans="2:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="87"/>
-      <c r="C29" s="160" t="s">
+      <c r="C29" s="150" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="160"/>
-      <c r="E29" s="160"/>
+      <c r="D29" s="150"/>
+      <c r="E29" s="150"/>
       <c r="F29" s="33"/>
-      <c r="G29" s="161" t="s">
+      <c r="G29" s="151" t="s">
         <v>59</v>
       </c>
-      <c r="H29" s="161"/>
-      <c r="I29" s="161"/>
-      <c r="J29" s="162" t="s">
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="152" t="s">
         <v>60</v>
       </c>
-      <c r="K29" s="163"/>
+      <c r="K29" s="153"/>
       <c r="L29" s="12" t="s">
         <v>61</v>
       </c>
@@ -3222,15 +3260,15 @@
     </row>
     <row r="30" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="87"/>
-      <c r="C30" s="160"/>
-      <c r="D30" s="160"/>
-      <c r="E30" s="160"/>
+      <c r="C30" s="150"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="150"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="164"/>
-      <c r="H30" s="165"/>
-      <c r="I30" s="166"/>
-      <c r="J30" s="167"/>
-      <c r="K30" s="168"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="155"/>
+      <c r="I30" s="156"/>
+      <c r="J30" s="157"/>
+      <c r="K30" s="158"/>
       <c r="L30" s="112"/>
       <c r="M30" s="113"/>
       <c r="N30" s="76"/>
@@ -3248,125 +3286,125 @@
       <c r="C32" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="169" t="s">
+      <c r="D32" s="136" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="169"/>
-      <c r="F32" s="169"/>
-      <c r="G32" s="169"/>
-      <c r="H32" s="169"/>
-      <c r="I32" s="169"/>
-      <c r="J32" s="169"/>
-      <c r="K32" s="169"/>
-      <c r="L32" s="169"/>
-      <c r="M32" s="169"/>
-      <c r="N32" s="169"/>
-      <c r="O32" s="169"/>
-      <c r="P32" s="169"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="136"/>
+      <c r="G32" s="136"/>
+      <c r="H32" s="136"/>
+      <c r="I32" s="136"/>
+      <c r="J32" s="136"/>
+      <c r="K32" s="136"/>
+      <c r="L32" s="136"/>
+      <c r="M32" s="136"/>
+      <c r="N32" s="136"/>
+      <c r="O32" s="136"/>
+      <c r="P32" s="136"/>
     </row>
     <row r="33" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C33" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="170"/>
-      <c r="E33" s="170"/>
-      <c r="F33" s="170"/>
-      <c r="G33" s="170"/>
-      <c r="H33" s="170"/>
-      <c r="I33" s="170"/>
-      <c r="J33" s="170"/>
-      <c r="K33" s="170"/>
-      <c r="L33" s="170"/>
-      <c r="M33" s="170"/>
-      <c r="N33" s="170"/>
-      <c r="O33" s="170"/>
-      <c r="P33" s="170"/>
+      <c r="D33" s="137"/>
+      <c r="E33" s="137"/>
+      <c r="F33" s="137"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="137"/>
+      <c r="I33" s="137"/>
+      <c r="J33" s="137"/>
+      <c r="K33" s="137"/>
+      <c r="L33" s="137"/>
+      <c r="M33" s="137"/>
+      <c r="N33" s="137"/>
+      <c r="O33" s="137"/>
+      <c r="P33" s="137"/>
     </row>
     <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
     </row>
     <row r="36" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="115" t="s">
+      <c r="C36" s="133" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="115"/>
-      <c r="E36" s="115"/>
-      <c r="F36" s="115"/>
-      <c r="G36" s="115"/>
+      <c r="D36" s="133"/>
+      <c r="E36" s="133"/>
+      <c r="F36" s="133"/>
+      <c r="G36" s="133"/>
       <c r="M36" s="77"/>
-      <c r="N36" s="115" t="s">
+      <c r="N36" s="133" t="s">
         <v>77</v>
       </c>
-      <c r="O36" s="115"/>
-      <c r="P36" s="115"/>
+      <c r="O36" s="133"/>
+      <c r="P36" s="133"/>
       <c r="Q36" s="98"/>
       <c r="R36" s="101"/>
     </row>
     <row r="37" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="137" t="s">
+      <c r="C37" s="179" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="137"/>
-      <c r="E37" s="137"/>
-      <c r="F37" s="137"/>
-      <c r="G37" s="137"/>
+      <c r="D37" s="179"/>
+      <c r="E37" s="179"/>
+      <c r="F37" s="179"/>
+      <c r="G37" s="179"/>
       <c r="M37" s="77"/>
-      <c r="N37" s="117" t="s">
+      <c r="N37" s="135" t="s">
         <v>76</v>
       </c>
-      <c r="O37" s="117"/>
-      <c r="P37" s="117"/>
+      <c r="O37" s="135"/>
+      <c r="P37" s="135"/>
       <c r="Q37" s="99"/>
       <c r="R37" s="101"/>
     </row>
     <row r="38" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="136" t="s">
+      <c r="C38" s="178" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="136"/>
-      <c r="E38" s="136"/>
-      <c r="F38" s="136"/>
-      <c r="G38" s="136"/>
+      <c r="D38" s="178"/>
+      <c r="E38" s="178"/>
+      <c r="F38" s="178"/>
+      <c r="G38" s="178"/>
       <c r="M38" s="77"/>
-      <c r="N38" s="136" t="s">
+      <c r="N38" s="178" t="s">
         <v>66</v>
       </c>
-      <c r="O38" s="136"/>
-      <c r="P38" s="136"/>
+      <c r="O38" s="178"/>
+      <c r="P38" s="178"/>
       <c r="Q38" s="100"/>
       <c r="R38" s="101"/>
     </row>
     <row r="39" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="136" t="s">
+      <c r="C39" s="178" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="136"/>
-      <c r="E39" s="136"/>
-      <c r="F39" s="136"/>
-      <c r="G39" s="136"/>
+      <c r="D39" s="178"/>
+      <c r="E39" s="178"/>
+      <c r="F39" s="178"/>
+      <c r="G39" s="178"/>
       <c r="M39" s="77"/>
-      <c r="N39" s="136" t="s">
+      <c r="N39" s="178" t="s">
         <v>32</v>
       </c>
-      <c r="O39" s="136"/>
-      <c r="P39" s="136"/>
+      <c r="O39" s="178"/>
+      <c r="P39" s="178"/>
       <c r="Q39" s="100"/>
       <c r="R39" s="101"/>
     </row>
     <row r="40" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="117" t="s">
+      <c r="C40" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="117"/>
-      <c r="E40" s="117"/>
-      <c r="F40" s="117"/>
-      <c r="G40" s="117"/>
+      <c r="D40" s="135"/>
+      <c r="E40" s="135"/>
+      <c r="F40" s="135"/>
+      <c r="G40" s="135"/>
       <c r="M40" s="77"/>
-      <c r="N40" s="117" t="s">
+      <c r="N40" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="O40" s="117"/>
-      <c r="P40" s="117"/>
+      <c r="O40" s="135"/>
+      <c r="P40" s="135"/>
       <c r="Q40" s="99"/>
       <c r="R40" s="101"/>
     </row>
@@ -3376,6 +3414,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="N40:P40"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="B21:P21"/>
+    <mergeCell ref="C23:E25"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="D32:P32"/>
     <mergeCell ref="D33:P33"/>
     <mergeCell ref="N36:P36"/>
@@ -3392,34 +3458,6 @@
     <mergeCell ref="I11:P12"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="B21:P21"/>
-    <mergeCell ref="C23:E25"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="N37:P37"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hot fix additional percentage
</commit_message>
<xml_diff>
--- a/creator/forms_xlsx/SBH-FORM.xlsx
+++ b/creator/forms_xlsx/SBH-FORM.xlsx
@@ -903,12 +903,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1264,6 +1265,60 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1274,59 +1329,140 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1336,146 +1472,49 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="34" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1758,7 +1797,9 @@
   </sheetPr>
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1769,7 +1810,7 @@
     <col min="6" max="6" width="26.28515625" style="77" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" style="77" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" style="77" customWidth="1"/>
-    <col min="9" max="9" width="10" style="77" customWidth="1"/>
+    <col min="9" max="9" width="10" style="194" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="117" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" style="77" customWidth="1"/>
     <col min="12" max="12" width="17.140625" style="77" customWidth="1"/>
@@ -1786,43 +1827,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="132" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
+      <c r="B1" s="129" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
+      <c r="P1" s="129"/>
       <c r="Q1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
       <c r="Q2" s="33"/>
     </row>
     <row r="3" spans="1:26" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1839,7 +1880,7 @@
       <c r="F4" s="94"/>
       <c r="G4" s="94"/>
       <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
+      <c r="I4" s="195"/>
       <c r="J4" s="118"/>
       <c r="K4" s="94"/>
       <c r="L4" s="94"/>
@@ -1928,7 +1969,7 @@
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
+      <c r="I8" s="196"/>
       <c r="J8" s="119"/>
       <c r="K8" s="28"/>
       <c r="L8" s="45"/>
@@ -1949,7 +1990,7 @@
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
+      <c r="I9" s="197"/>
       <c r="J9" s="120"/>
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
@@ -1963,68 +2004,68 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="141" t="s">
+      <c r="B10" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="142"/>
-      <c r="D10" s="142"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="142"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="142"/>
-      <c r="I10" s="143"/>
-      <c r="J10" s="135" t="s">
+      <c r="C10" s="139"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="140"/>
+      <c r="J10" s="132" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="135"/>
-      <c r="L10" s="135"/>
-      <c r="M10" s="135"/>
-      <c r="N10" s="135"/>
-      <c r="O10" s="135"/>
-      <c r="P10" s="135"/>
+      <c r="K10" s="132"/>
+      <c r="L10" s="132"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
+      <c r="O10" s="132"/>
+      <c r="P10" s="132"/>
       <c r="Q10" s="33"/>
       <c r="Z10" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="144"/>
-      <c r="C11" s="145"/>
-      <c r="D11" s="145"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="145"/>
-      <c r="G11" s="145"/>
-      <c r="H11" s="145"/>
-      <c r="I11" s="146"/>
-      <c r="J11" s="136"/>
-      <c r="K11" s="136"/>
-      <c r="L11" s="136"/>
-      <c r="M11" s="136"/>
-      <c r="N11" s="136"/>
-      <c r="O11" s="136"/>
-      <c r="P11" s="136"/>
+      <c r="B11" s="141"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="142"/>
+      <c r="E11" s="142"/>
+      <c r="F11" s="142"/>
+      <c r="G11" s="142"/>
+      <c r="H11" s="142"/>
+      <c r="I11" s="143"/>
+      <c r="J11" s="133"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="133"/>
+      <c r="M11" s="133"/>
+      <c r="N11" s="133"/>
+      <c r="O11" s="133"/>
+      <c r="P11" s="133"/>
       <c r="Q11" s="33"/>
       <c r="Z11" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="148"/>
-      <c r="D12" s="148"/>
-      <c r="E12" s="148"/>
-      <c r="F12" s="148"/>
-      <c r="G12" s="148"/>
-      <c r="H12" s="148"/>
-      <c r="I12" s="148"/>
-      <c r="J12" s="148"/>
-      <c r="K12" s="148"/>
-      <c r="L12" s="148"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
-      <c r="O12" s="149"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="145"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="145"/>
+      <c r="K12" s="145"/>
+      <c r="L12" s="145"/>
+      <c r="M12" s="145"/>
+      <c r="N12" s="145"/>
+      <c r="O12" s="146"/>
       <c r="P12" s="29" t="s">
         <v>5</v>
       </c>
@@ -2055,7 +2096,7 @@
       <c r="H13" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="92" t="s">
+      <c r="I13" s="198" t="s">
         <v>72</v>
       </c>
       <c r="J13" s="121" t="s">
@@ -2106,7 +2147,7 @@
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
+      <c r="I14" s="199"/>
       <c r="J14" s="122"/>
       <c r="K14" s="65"/>
       <c r="L14" s="65"/>
@@ -2157,7 +2198,7 @@
       <c r="H15" s="65">
         <v>6</v>
       </c>
-      <c r="I15" s="65">
+      <c r="I15" s="199">
         <v>7</v>
       </c>
       <c r="J15" s="122">
@@ -2211,7 +2252,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="17"/>
+      <c r="I16" s="200"/>
       <c r="J16" s="17"/>
       <c r="K16" s="5"/>
       <c r="L16" s="53"/>
@@ -2244,13 +2285,13 @@
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="137" t="s">
+      <c r="E17" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="138"/>
+      <c r="F17" s="135"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
+      <c r="I17" s="201"/>
       <c r="J17" s="123"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
@@ -2287,7 +2328,7 @@
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
-      <c r="I18" s="43"/>
+      <c r="I18" s="202"/>
       <c r="J18" s="124"/>
       <c r="K18" s="43"/>
       <c r="L18" s="43"/>
@@ -2324,7 +2365,7 @@
       <c r="F19" s="32"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
-      <c r="I19" s="43"/>
+      <c r="I19" s="202"/>
       <c r="J19" s="124"/>
       <c r="K19" s="43"/>
       <c r="L19" s="43"/>
@@ -2361,7 +2402,7 @@
       <c r="F20" s="89"/>
       <c r="G20" s="89"/>
       <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
+      <c r="I20" s="203"/>
       <c r="J20" s="125"/>
       <c r="K20" s="89"/>
       <c r="L20" s="89"/>
@@ -2398,7 +2439,7 @@
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
+      <c r="I21" s="204"/>
       <c r="J21" s="126"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
@@ -2412,15 +2453,15 @@
       </c>
     </row>
     <row r="22" spans="1:26" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="139"/>
-      <c r="B22" s="140"/>
-      <c r="C22" s="140"/>
-      <c r="D22" s="140"/>
-      <c r="E22" s="140"/>
+      <c r="A22" s="136"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
+      <c r="I22" s="197"/>
       <c r="J22" s="120"/>
       <c r="K22" s="33"/>
       <c r="L22" s="6"/>
@@ -2440,12 +2481,12 @@
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="129" t="s">
+      <c r="B24" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
+      <c r="C24" s="147"/>
+      <c r="D24" s="147"/>
+      <c r="E24" s="147"/>
       <c r="L24" s="101"/>
       <c r="M24" s="98"/>
       <c r="N24" s="98"/>
@@ -2453,12 +2494,12 @@
       <c r="P24" s="98"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B25" s="130" t="s">
+      <c r="B25" s="148" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="130"/>
-      <c r="D25" s="130"/>
-      <c r="E25" s="130"/>
+      <c r="C25" s="148"/>
+      <c r="D25" s="148"/>
+      <c r="E25" s="148"/>
       <c r="L25" s="101"/>
       <c r="M25" s="100"/>
       <c r="N25" s="100"/>
@@ -2469,12 +2510,13 @@
       </c>
     </row>
     <row r="26" spans="1:26" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="131" t="s">
+      <c r="B26" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="131"/>
-      <c r="D26" s="131"/>
-      <c r="E26" s="131"/>
+      <c r="C26" s="149"/>
+      <c r="D26" s="149"/>
+      <c r="E26" s="149"/>
+      <c r="I26" s="205"/>
       <c r="J26" s="127"/>
       <c r="L26" s="96"/>
       <c r="M26" s="99"/>
@@ -2484,12 +2526,13 @@
       <c r="U26" s="102"/>
     </row>
     <row r="27" spans="1:26" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="131" t="s">
+      <c r="B27" s="149" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="131"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
+      <c r="C27" s="149"/>
+      <c r="D27" s="149"/>
+      <c r="E27" s="149"/>
+      <c r="I27" s="205"/>
       <c r="J27" s="127"/>
       <c r="L27" s="96"/>
       <c r="M27" s="99"/>
@@ -2499,12 +2542,13 @@
       <c r="U27" s="102"/>
     </row>
     <row r="28" spans="1:26" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="131" t="s">
+      <c r="B28" s="149" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="131"/>
-      <c r="D28" s="131"/>
-      <c r="E28" s="131"/>
+      <c r="C28" s="149"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="149"/>
+      <c r="I28" s="205"/>
       <c r="J28" s="127"/>
       <c r="L28" s="96"/>
       <c r="M28" s="99"/>
@@ -2528,11 +2572,16 @@
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
+      <c r="I34" s="206"/>
       <c r="J34" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="J10:P11"/>
@@ -2540,11 +2589,6 @@
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="B10:I11"/>
     <mergeCell ref="B12:O12"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2587,23 +2631,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="129" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
+      <c r="P1" s="129"/>
       <c r="Q1" s="33"/>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2625,23 +2669,23 @@
       <c r="Q2" s="33"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="162" t="s">
+      <c r="B3" s="152" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
-      <c r="M3" s="162"/>
-      <c r="N3" s="162"/>
-      <c r="O3" s="162"/>
-      <c r="P3" s="162"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
+      <c r="L3" s="152"/>
+      <c r="M3" s="152"/>
+      <c r="N3" s="152"/>
+      <c r="O3" s="152"/>
+      <c r="P3" s="152"/>
       <c r="Q3" s="33"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2733,14 +2777,14 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11"/>
-      <c r="C8" s="187"/>
-      <c r="D8" s="187"/>
-      <c r="E8" s="187"/>
-      <c r="F8" s="188"/>
-      <c r="G8" s="188"/>
+      <c r="C8" s="155"/>
+      <c r="D8" s="155"/>
+      <c r="E8" s="155"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="156"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="188"/>
-      <c r="J8" s="188"/>
+      <c r="I8" s="156"/>
+      <c r="J8" s="156"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="37"/>
@@ -2786,91 +2830,91 @@
       <c r="Q10" s="33"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="189" t="str">
+      <c r="B11" s="157" t="str">
         <f>'SBH-FORM 1'!B10</f>
         <v xml:space="preserve">Outsource Service Description : </v>
       </c>
-      <c r="C11" s="190"/>
-      <c r="D11" s="190"/>
-      <c r="E11" s="190"/>
-      <c r="F11" s="190"/>
-      <c r="G11" s="190"/>
-      <c r="H11" s="190"/>
-      <c r="I11" s="190" t="str">
+      <c r="C11" s="158"/>
+      <c r="D11" s="158"/>
+      <c r="E11" s="158"/>
+      <c r="F11" s="158"/>
+      <c r="G11" s="158"/>
+      <c r="H11" s="158"/>
+      <c r="I11" s="158" t="str">
         <f>'SBH-FORM 1'!J10</f>
         <v>Team Based Hiring for Division Name</v>
       </c>
-      <c r="J11" s="190"/>
-      <c r="K11" s="190"/>
-      <c r="L11" s="190"/>
-      <c r="M11" s="190"/>
-      <c r="N11" s="191"/>
-      <c r="O11" s="191"/>
-      <c r="P11" s="192"/>
+      <c r="J11" s="158"/>
+      <c r="K11" s="158"/>
+      <c r="L11" s="158"/>
+      <c r="M11" s="158"/>
+      <c r="N11" s="159"/>
+      <c r="O11" s="159"/>
+      <c r="P11" s="160"/>
       <c r="Q11" s="33"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="185"/>
-      <c r="C12" s="186"/>
-      <c r="D12" s="186"/>
-      <c r="E12" s="186"/>
-      <c r="F12" s="186"/>
-      <c r="G12" s="186"/>
-      <c r="H12" s="186"/>
-      <c r="I12" s="186"/>
-      <c r="J12" s="186"/>
-      <c r="K12" s="186"/>
-      <c r="L12" s="186"/>
-      <c r="M12" s="186"/>
-      <c r="N12" s="193"/>
-      <c r="O12" s="193"/>
-      <c r="P12" s="156"/>
+      <c r="B12" s="153"/>
+      <c r="C12" s="154"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="154"/>
+      <c r="F12" s="154"/>
+      <c r="G12" s="154"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
+      <c r="K12" s="154"/>
+      <c r="L12" s="154"/>
+      <c r="M12" s="154"/>
+      <c r="N12" s="161"/>
+      <c r="O12" s="161"/>
+      <c r="P12" s="162"/>
       <c r="Q12" s="33"/>
     </row>
     <row r="13" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="185" t="s">
+      <c r="B13" s="153" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="186" t="s">
+      <c r="C13" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="186" t="s">
+      <c r="D13" s="154" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="186"/>
-      <c r="F13" s="186"/>
-      <c r="G13" s="186" t="s">
+      <c r="E13" s="154"/>
+      <c r="F13" s="154"/>
+      <c r="G13" s="154" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="186"/>
-      <c r="I13" s="186"/>
-      <c r="J13" s="186" t="s">
+      <c r="H13" s="154"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="186"/>
-      <c r="L13" s="186"/>
-      <c r="M13" s="155" t="s">
+      <c r="K13" s="154"/>
+      <c r="L13" s="154"/>
+      <c r="M13" s="163" t="s">
         <v>42</v>
       </c>
-      <c r="N13" s="155" t="s">
+      <c r="N13" s="163" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="155" t="s">
+      <c r="O13" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="P13" s="156" t="s">
+      <c r="P13" s="162" t="s">
         <v>17</v>
       </c>
       <c r="Q13" s="33"/>
-      <c r="R13" s="152">
+      <c r="R13" s="186">
         <v>180</v>
       </c>
-      <c r="S13" s="153"/>
-      <c r="T13" s="154"/>
+      <c r="S13" s="187"/>
+      <c r="T13" s="188"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="185"/>
-      <c r="C14" s="186"/>
+      <c r="B14" s="153"/>
+      <c r="C14" s="154"/>
       <c r="D14" s="92" t="s">
         <v>44</v>
       </c>
@@ -2898,10 +2942,10 @@
       <c r="L14" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="M14" s="155"/>
-      <c r="N14" s="155"/>
-      <c r="O14" s="155"/>
-      <c r="P14" s="156"/>
+      <c r="M14" s="163"/>
+      <c r="N14" s="163"/>
+      <c r="O14" s="163"/>
+      <c r="P14" s="162"/>
       <c r="Q14" s="33"/>
       <c r="R14" s="34" t="s">
         <v>21</v>
@@ -3039,17 +3083,17 @@
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B18" s="157"/>
-      <c r="C18" s="158"/>
-      <c r="D18" s="158"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
-      <c r="K18" s="158"/>
-      <c r="L18" s="159"/>
+      <c r="B18" s="189"/>
+      <c r="C18" s="190"/>
+      <c r="D18" s="190"/>
+      <c r="E18" s="190"/>
+      <c r="F18" s="190"/>
+      <c r="G18" s="190"/>
+      <c r="H18" s="190"/>
+      <c r="I18" s="190"/>
+      <c r="J18" s="190"/>
+      <c r="K18" s="190"/>
+      <c r="L18" s="191"/>
       <c r="M18" s="44"/>
       <c r="N18" s="73" t="s">
         <v>47</v>
@@ -3065,24 +3109,24 @@
       </c>
     </row>
     <row r="19" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="166" t="s">
+      <c r="B19" s="178" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="167"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="171"/>
-      <c r="F19" s="171"/>
-      <c r="G19" s="172">
+      <c r="C19" s="179"/>
+      <c r="D19" s="183"/>
+      <c r="E19" s="183"/>
+      <c r="F19" s="183"/>
+      <c r="G19" s="184">
         <f>COUNTIF('SBH-FORM 1'!U:U, "YES")</f>
         <v>0</v>
       </c>
-      <c r="H19" s="172"/>
-      <c r="I19" s="172"/>
-      <c r="J19" s="173">
+      <c r="H19" s="184"/>
+      <c r="I19" s="184"/>
+      <c r="J19" s="185">
         <v>160</v>
       </c>
-      <c r="K19" s="173"/>
-      <c r="L19" s="173"/>
+      <c r="K19" s="185"/>
+      <c r="L19" s="185"/>
       <c r="M19" s="48"/>
       <c r="N19" s="74"/>
       <c r="O19" s="80">
@@ -3105,10 +3149,10 @@
       <c r="H20" s="33"/>
       <c r="I20" s="33"/>
       <c r="J20" s="15"/>
-      <c r="M20" s="160" t="s">
+      <c r="M20" s="173" t="s">
         <v>49</v>
       </c>
-      <c r="N20" s="161"/>
+      <c r="N20" s="174"/>
       <c r="O20" s="103" t="e">
         <f ca="1">INDIRECT("O"&amp;ROW()-2)-INDIRECT("O"&amp;ROW()-1)</f>
         <v>#N/A</v>
@@ -3116,23 +3160,23 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="162" t="s">
+      <c r="B21" s="152" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="162"/>
-      <c r="D21" s="162"/>
-      <c r="E21" s="162"/>
-      <c r="F21" s="162"/>
-      <c r="G21" s="162"/>
-      <c r="H21" s="162"/>
-      <c r="I21" s="162"/>
-      <c r="J21" s="162"/>
-      <c r="K21" s="162"/>
-      <c r="L21" s="162"/>
-      <c r="M21" s="162"/>
-      <c r="N21" s="162"/>
-      <c r="O21" s="162"/>
-      <c r="P21" s="162"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="152"/>
+      <c r="G21" s="152"/>
+      <c r="H21" s="152"/>
+      <c r="I21" s="152"/>
+      <c r="J21" s="152"/>
+      <c r="K21" s="152"/>
+      <c r="L21" s="152"/>
+      <c r="M21" s="152"/>
+      <c r="N21" s="152"/>
+      <c r="O21" s="152"/>
+      <c r="P21" s="152"/>
       <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3155,11 +3199,11 @@
     </row>
     <row r="23" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
-      <c r="C23" s="163" t="s">
+      <c r="C23" s="175" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="164"/>
-      <c r="E23" s="164"/>
+      <c r="D23" s="176"/>
+      <c r="E23" s="176"/>
       <c r="F23" s="33"/>
       <c r="G23" s="33"/>
       <c r="H23" s="33"/>
@@ -3179,9 +3223,9 @@
     </row>
     <row r="24" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
-      <c r="C24" s="164"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="164"/>
+      <c r="C24" s="176"/>
+      <c r="D24" s="176"/>
+      <c r="E24" s="176"/>
       <c r="F24" s="33"/>
       <c r="G24" s="33"/>
       <c r="H24" s="33"/>
@@ -3197,9 +3241,9 @@
     </row>
     <row r="25" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="33"/>
-      <c r="C25" s="164"/>
-      <c r="D25" s="164"/>
-      <c r="E25" s="164"/>
+      <c r="C25" s="176"/>
+      <c r="D25" s="176"/>
+      <c r="E25" s="176"/>
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
       <c r="H25" s="33"/>
@@ -3238,14 +3282,14 @@
     <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="87"/>
       <c r="F27" s="33"/>
-      <c r="G27" s="165" t="s">
+      <c r="G27" s="177" t="s">
         <v>56</v>
       </c>
-      <c r="H27" s="165"/>
-      <c r="I27" s="165"/>
-      <c r="J27" s="168"/>
-      <c r="K27" s="169"/>
-      <c r="L27" s="170"/>
+      <c r="H27" s="177"/>
+      <c r="I27" s="177"/>
+      <c r="J27" s="180"/>
+      <c r="K27" s="181"/>
+      <c r="L27" s="182"/>
       <c r="M27" s="38"/>
       <c r="N27" s="38"/>
       <c r="O27" s="38"/>
@@ -3269,21 +3313,21 @@
     </row>
     <row r="29" spans="2:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="87"/>
-      <c r="C29" s="174" t="s">
+      <c r="C29" s="164" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="174"/>
-      <c r="E29" s="174"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="164"/>
       <c r="F29" s="33"/>
-      <c r="G29" s="175" t="s">
+      <c r="G29" s="165" t="s">
         <v>58</v>
       </c>
-      <c r="H29" s="175"/>
-      <c r="I29" s="175"/>
-      <c r="J29" s="176" t="s">
+      <c r="H29" s="165"/>
+      <c r="I29" s="165"/>
+      <c r="J29" s="166" t="s">
         <v>59</v>
       </c>
-      <c r="K29" s="177"/>
+      <c r="K29" s="167"/>
       <c r="L29" s="12" t="s">
         <v>60</v>
       </c>
@@ -3297,15 +3341,15 @@
     </row>
     <row r="30" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="87"/>
-      <c r="C30" s="174"/>
-      <c r="D30" s="174"/>
-      <c r="E30" s="174"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="164"/>
+      <c r="E30" s="164"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="178"/>
-      <c r="H30" s="179"/>
-      <c r="I30" s="180"/>
-      <c r="J30" s="181"/>
-      <c r="K30" s="182"/>
+      <c r="G30" s="168"/>
+      <c r="H30" s="169"/>
+      <c r="I30" s="170"/>
+      <c r="J30" s="171"/>
+      <c r="K30" s="172"/>
       <c r="L30" s="112"/>
       <c r="M30" s="113"/>
       <c r="N30" s="76"/>
@@ -3323,125 +3367,125 @@
       <c r="C32" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="183" t="s">
+      <c r="D32" s="150" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="183"/>
-      <c r="F32" s="183"/>
-      <c r="G32" s="183"/>
-      <c r="H32" s="183"/>
-      <c r="I32" s="183"/>
-      <c r="J32" s="183"/>
-      <c r="K32" s="183"/>
-      <c r="L32" s="183"/>
-      <c r="M32" s="183"/>
-      <c r="N32" s="183"/>
-      <c r="O32" s="183"/>
-      <c r="P32" s="183"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="150"/>
+      <c r="H32" s="150"/>
+      <c r="I32" s="150"/>
+      <c r="J32" s="150"/>
+      <c r="K32" s="150"/>
+      <c r="L32" s="150"/>
+      <c r="M32" s="150"/>
+      <c r="N32" s="150"/>
+      <c r="O32" s="150"/>
+      <c r="P32" s="150"/>
     </row>
     <row r="33" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C33" s="114" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="184"/>
-      <c r="E33" s="184"/>
-      <c r="F33" s="184"/>
-      <c r="G33" s="184"/>
-      <c r="H33" s="184"/>
-      <c r="I33" s="184"/>
-      <c r="J33" s="184"/>
-      <c r="K33" s="184"/>
-      <c r="L33" s="184"/>
-      <c r="M33" s="184"/>
-      <c r="N33" s="184"/>
-      <c r="O33" s="184"/>
-      <c r="P33" s="184"/>
+      <c r="D33" s="151"/>
+      <c r="E33" s="151"/>
+      <c r="F33" s="151"/>
+      <c r="G33" s="151"/>
+      <c r="H33" s="151"/>
+      <c r="I33" s="151"/>
+      <c r="J33" s="151"/>
+      <c r="K33" s="151"/>
+      <c r="L33" s="151"/>
+      <c r="M33" s="151"/>
+      <c r="N33" s="151"/>
+      <c r="O33" s="151"/>
+      <c r="P33" s="151"/>
     </row>
     <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
     </row>
     <row r="36" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="129" t="s">
+      <c r="C36" s="147" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="129"/>
-      <c r="E36" s="129"/>
-      <c r="F36" s="129"/>
-      <c r="G36" s="129"/>
+      <c r="D36" s="147"/>
+      <c r="E36" s="147"/>
+      <c r="F36" s="147"/>
+      <c r="G36" s="147"/>
       <c r="M36" s="77"/>
-      <c r="N36" s="129" t="s">
+      <c r="N36" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="O36" s="129"/>
-      <c r="P36" s="129"/>
+      <c r="O36" s="147"/>
+      <c r="P36" s="147"/>
       <c r="Q36" s="98"/>
       <c r="R36" s="101"/>
     </row>
     <row r="37" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="151" t="s">
+      <c r="C37" s="193" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="151"/>
-      <c r="E37" s="151"/>
-      <c r="F37" s="151"/>
-      <c r="G37" s="151"/>
+      <c r="D37" s="193"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193"/>
       <c r="M37" s="77"/>
-      <c r="N37" s="131" t="s">
+      <c r="N37" s="149" t="s">
         <v>75</v>
       </c>
-      <c r="O37" s="131"/>
-      <c r="P37" s="131"/>
+      <c r="O37" s="149"/>
+      <c r="P37" s="149"/>
       <c r="Q37" s="99"/>
       <c r="R37" s="101"/>
     </row>
     <row r="38" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="150" t="s">
+      <c r="C38" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="150"/>
-      <c r="E38" s="150"/>
-      <c r="F38" s="150"/>
-      <c r="G38" s="150"/>
+      <c r="D38" s="192"/>
+      <c r="E38" s="192"/>
+      <c r="F38" s="192"/>
+      <c r="G38" s="192"/>
       <c r="M38" s="77"/>
-      <c r="N38" s="150" t="s">
+      <c r="N38" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="O38" s="150"/>
-      <c r="P38" s="150"/>
+      <c r="O38" s="192"/>
+      <c r="P38" s="192"/>
       <c r="Q38" s="100"/>
       <c r="R38" s="101"/>
     </row>
     <row r="39" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="150" t="s">
+      <c r="C39" s="192" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="150"/>
-      <c r="E39" s="150"/>
-      <c r="F39" s="150"/>
-      <c r="G39" s="150"/>
+      <c r="D39" s="192"/>
+      <c r="E39" s="192"/>
+      <c r="F39" s="192"/>
+      <c r="G39" s="192"/>
       <c r="M39" s="77"/>
-      <c r="N39" s="150" t="s">
+      <c r="N39" s="192" t="s">
         <v>31</v>
       </c>
-      <c r="O39" s="150"/>
-      <c r="P39" s="150"/>
+      <c r="O39" s="192"/>
+      <c r="P39" s="192"/>
       <c r="Q39" s="100"/>
       <c r="R39" s="101"/>
     </row>
     <row r="40" spans="3:18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="131" t="s">
+      <c r="C40" s="149" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="131"/>
-      <c r="E40" s="131"/>
-      <c r="F40" s="131"/>
-      <c r="G40" s="131"/>
+      <c r="D40" s="149"/>
+      <c r="E40" s="149"/>
+      <c r="F40" s="149"/>
+      <c r="G40" s="149"/>
       <c r="M40" s="77"/>
-      <c r="N40" s="131" t="s">
+      <c r="N40" s="149" t="s">
         <v>32</v>
       </c>
-      <c r="O40" s="131"/>
-      <c r="P40" s="131"/>
+      <c r="O40" s="149"/>
+      <c r="P40" s="149"/>
       <c r="Q40" s="99"/>
       <c r="R40" s="101"/>
     </row>
@@ -3451,6 +3495,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="N40:P40"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="B21:P21"/>
+    <mergeCell ref="C23:E25"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="D32:P32"/>
     <mergeCell ref="D33:P33"/>
     <mergeCell ref="N36:P36"/>
@@ -3467,34 +3539,6 @@
     <mergeCell ref="I11:P12"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="B21:P21"/>
-    <mergeCell ref="C23:E25"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="N37:P37"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>